<commit_message>
fixes parrott -> parrot typos
</commit_message>
<xml_diff>
--- a/data-raw/metadata/butte_release_metadata.xlsx
+++ b/data-raw/metadata/butte_release_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-butte-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B102E10A-F0BC-774F-925B-CC8B055513DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B078F08-5F38-C844-8066-D2B90F18A40D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -199,9 +199,6 @@
     <t>Origin or production type of fish marked. Levels = c("Natural", NA)</t>
   </si>
   <si>
-    <t>Site where fish used for release were from. Levels = c("Parrott-Phelan canal trap box", NA, "Parrot-Phelan RST").</t>
-  </si>
-  <si>
     <t>Site where fish were released. Levels = c("Not applicable", "Parrott-Phelan e-test release site").</t>
   </si>
   <si>
@@ -215,6 +212,9 @@
   </si>
   <si>
     <t>Whether or not to include data in analysis. Levels = c("Yes", "No", NA).</t>
+  </si>
+  <si>
+    <t>Site where fish used for release were from. Levels = c("Parrot-Phelan canal trap box", NA, "Parrot-Phelan RST").</t>
   </si>
 </sst>
 </file>
@@ -283,7 +283,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -317,11 +317,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,7 +535,7 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -847,7 +842,7 @@
         <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>14</v>
@@ -885,7 +880,7 @@
         <v>26</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>14</v>
@@ -935,7 +930,7 @@
         <v>20</v>
       </c>
       <c r="F10" s="3"/>
-      <c r="G10" s="18"/>
+      <c r="G10" s="9"/>
       <c r="H10" s="3"/>
       <c r="I10" s="2"/>
       <c r="J10" s="3"/>
@@ -956,53 +951,53 @@
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
     </row>
-    <row r="11" spans="1:26" s="21" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="17" t="s">
+    <row r="11" spans="1:26" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="E11" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="18" t="s">
+      <c r="F11" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G11" s="18" t="s">
+      <c r="G11" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="H11" s="18" t="s">
+      <c r="H11" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="I11" s="20"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="18">
+      <c r="I11" s="10"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="9">
         <v>100</v>
       </c>
-      <c r="M11" s="18">
+      <c r="M11" s="9">
         <v>500</v>
       </c>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="17"/>
-      <c r="Q11" s="17"/>
-      <c r="R11" s="17"/>
-      <c r="S11" s="17"/>
-      <c r="T11" s="17"/>
-      <c r="U11" s="17"/>
-      <c r="V11" s="17"/>
-      <c r="W11" s="17"/>
-      <c r="X11" s="17"/>
-      <c r="Y11" s="17"/>
-      <c r="Z11" s="17"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4"/>
+      <c r="V11" s="4"/>
+      <c r="W11" s="4"/>
+      <c r="X11" s="4"/>
+      <c r="Y11" s="4"/>
+      <c r="Z11" s="4"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
@@ -1048,60 +1043,60 @@
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
     </row>
-    <row r="13" spans="1:26" s="21" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="17" t="s">
+    <row r="13" spans="1:26" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="E13" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G13" s="18" t="s">
+      <c r="G13" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="H13" s="18" t="s">
+      <c r="H13" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="I13" s="20"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="18">
+      <c r="I13" s="10"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="9">
         <v>6</v>
       </c>
-      <c r="M13" s="18">
+      <c r="M13" s="9">
         <v>7</v>
       </c>
-      <c r="N13" s="17"/>
-      <c r="O13" s="17"/>
-      <c r="P13" s="17"/>
-      <c r="Q13" s="17"/>
-      <c r="R13" s="17"/>
-      <c r="S13" s="17"/>
-      <c r="T13" s="17"/>
-      <c r="U13" s="17"/>
-      <c r="V13" s="17"/>
-      <c r="W13" s="17"/>
-      <c r="X13" s="17"/>
-      <c r="Y13" s="17"/>
-      <c r="Z13" s="17"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4"/>
+      <c r="V13" s="4"/>
+      <c r="W13" s="4"/>
+      <c r="X13" s="4"/>
+      <c r="Y13" s="4"/>
+      <c r="Z13" s="4"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>41</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>14</v>
@@ -1139,7 +1134,7 @@
         <v>42</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>14</v>
@@ -1177,7 +1172,7 @@
         <v>43</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>14</v>
@@ -1253,7 +1248,7 @@
         <v>51</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
standardizes Parrott to Parrot and rewrites xml
</commit_message>
<xml_diff>
--- a/data-raw/metadata/butte_release_metadata.xlsx
+++ b/data-raw/metadata/butte_release_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-butte-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B078F08-5F38-C844-8066-D2B90F18A40D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE95C1B-3D48-DA41-8D4B-EA747EC2ADBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -199,9 +199,6 @@
     <t>Origin or production type of fish marked. Levels = c("Natural", NA)</t>
   </si>
   <si>
-    <t>Site where fish were released. Levels = c("Not applicable", "Parrott-Phelan e-test release site").</t>
-  </si>
-  <si>
     <t>Mark type that was applied to the release group. Levels = c("Pigment / dye", NA)</t>
   </si>
   <si>
@@ -215,6 +212,9 @@
   </si>
   <si>
     <t>Site where fish used for release were from. Levels = c("Parrot-Phelan canal trap box", NA, "Parrot-Phelan RST").</t>
+  </si>
+  <si>
+    <t>Site where fish were released. Levels = c("Not applicable", "Parrot-Phelan e-test release site").</t>
   </si>
 </sst>
 </file>
@@ -535,7 +535,7 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -842,7 +842,7 @@
         <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>14</v>
@@ -880,7 +880,7 @@
         <v>26</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>14</v>
@@ -1096,7 +1096,7 @@
         <v>41</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>14</v>
@@ -1134,7 +1134,7 @@
         <v>42</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>14</v>
@@ -1172,7 +1172,7 @@
         <v>43</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>14</v>
@@ -1248,7 +1248,7 @@
         <v>51</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>14</v>

</xml_diff>